<commit_message>
Move initialization warnings into error message so they don't get printed if the error is caught
</commit_message>
<xml_diff>
--- a/atomica/library/hypertension_framework.xlsx
+++ b/atomica/library/hypertension_framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\atomica\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3770DB6-9E62-46C7-8F6C-3AA2B62E8681}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2571B7CD-E242-48FB-9179-65342C872F6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,14 @@
     <sheet name="Characteristics" sheetId="5" r:id="rId5"/>
     <sheet name="Parameters" sheetId="6" r:id="rId6"/>
     <sheet name="Cascades" sheetId="7" r:id="rId7"/>
+    <sheet name="Plots" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -551,8 +553,45 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>None</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{DFFDD34D-F360-49F0-8EAC-F9F63BC6CD25}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This column is for the 'display name' of a compartment within a
+population cascade, a state that an entity can exist in that is
+distinct from all other states.
+Examples may include 'Susceptible', 'Infected Stage 1', 'Recovered',
+etc.
+If entities in the network involve two 'orthogonal' descriptors,
+compartments should combine the status of each state in the title,
+e.g. 'High Income Earner + Year 12 Education', to make sure that each
+entity in a cascade is only ever in one state at a time.
+It is possible to bundle independent states as analytical features of
+interest elsewhere in the framework file.
+Note: A display name is a representative label that users interface
+with (e.g. in databooks and plots).
+It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -815,13 +854,34 @@
     <t>Treatment failure rate</t>
   </si>
   <si>
-    <t>main</t>
-  </si>
-  <si>
     <t>Constituents</t>
   </si>
   <si>
     <t>Prevalent</t>
+  </si>
+  <si>
+    <t>Quantities</t>
+  </si>
+  <si>
+    <t>Undiagnosed compartment</t>
+  </si>
+  <si>
+    <t>Screened compartment</t>
+  </si>
+  <si>
+    <t>Diagnosed compartment</t>
+  </si>
+  <si>
+    <t>Treated compartment</t>
+  </si>
+  <si>
+    <t>Controlled compartment</t>
+  </si>
+  <si>
+    <t>Treatment only</t>
+  </si>
+  <si>
+    <t>All stages</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1470,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,11 +2203,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2157,15 +2215,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>48</v>
@@ -2203,7 +2261,111 @@
         <v>60</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1138990-DC73-4184-AF4A-CCEB4A7F8BAA}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>